<commit_message>
Remove 930 and E01/E02
</commit_message>
<xml_diff>
--- a/output/current_sector_analysis.xlsx
+++ b/output/current_sector_analysis.xlsx
@@ -572,21 +572,21 @@
     <t xml:space="preserve">Algeria</t>
   </si>
   <si>
+    <t xml:space="preserve">Kosovo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Iran</t>
   </si>
   <si>
-    <t xml:space="preserve">Kosovo</t>
+    <t xml:space="preserve">Vanuatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azerbaijan</t>
   </si>
   <si>
     <t xml:space="preserve">Venezuela</t>
   </si>
   <si>
-    <t xml:space="preserve">Vanuatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azerbaijan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tuvalu</t>
   </si>
   <si>
@@ -596,28 +596,28 @@
     <t xml:space="preserve">Palau</t>
   </si>
   <si>
+    <t xml:space="preserve">Caribbean, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sudan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equatorial Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Asia, regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauritius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic People's Republic of Korea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liberia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caribbean, regional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Sudan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equatorial Guinea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Asia, regional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mauritius</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Democratic People's Republic of Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo</t>
   </si>
   <si>
     <t xml:space="preserve">Central African Republic</t>
@@ -1211,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>629.513244</v>
+        <v>629.475001</v>
       </c>
     </row>
     <row r="4">
@@ -1298,7 +1298,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>93.731078</v>
+        <v>93.720986</v>
       </c>
     </row>
     <row r="9">
@@ -1410,7 +1410,7 @@
         <v>26</v>
       </c>
       <c r="B22" t="n">
-        <v>6.523764</v>
+        <v>6.495613</v>
       </c>
     </row>
     <row r="23">
@@ -1673,7 +1673,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="n">
-        <v>1063.00181293564</v>
+        <v>1062.99394373859</v>
       </c>
     </row>
     <row r="3">
@@ -1681,7 +1681,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="n">
-        <v>562.979409386849</v>
+        <v>562.954186595814</v>
       </c>
     </row>
     <row r="4">
@@ -1689,7 +1689,7 @@
         <v>59</v>
       </c>
       <c r="B4" t="n">
-        <v>276.380938352018</v>
+        <v>276.016562146275</v>
       </c>
     </row>
     <row r="5">
@@ -1697,7 +1697,7 @@
         <v>60</v>
       </c>
       <c r="B5" t="n">
-        <v>227.203115344336</v>
+        <v>227.203524254056</v>
       </c>
     </row>
     <row r="6">
@@ -1705,7 +1705,7 @@
         <v>61</v>
       </c>
       <c r="B6" t="n">
-        <v>3.6279573246119</v>
+        <v>3.62807467954036</v>
       </c>
     </row>
   </sheetData>
@@ -1736,7 +1736,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="n">
-        <v>218.593888046866</v>
+        <v>218.59391310176</v>
       </c>
     </row>
     <row r="3">
@@ -1744,7 +1744,7 @@
         <v>64</v>
       </c>
       <c r="B3" t="n">
-        <v>188.466295499605</v>
+        <v>188.466403893866</v>
       </c>
     </row>
     <row r="4">
@@ -1752,7 +1752,7 @@
         <v>65</v>
       </c>
       <c r="B4" t="n">
-        <v>157.951849819173</v>
+        <v>157.951720453064</v>
       </c>
     </row>
     <row r="5">
@@ -1760,7 +1760,7 @@
         <v>66</v>
       </c>
       <c r="B5" t="n">
-        <v>141.053898053115</v>
+        <v>141.053879741973</v>
       </c>
     </row>
     <row r="6">
@@ -1768,7 +1768,7 @@
         <v>67</v>
       </c>
       <c r="B6" t="n">
-        <v>118.929576316368</v>
+        <v>118.929148581731</v>
       </c>
     </row>
     <row r="7">
@@ -1776,7 +1776,7 @@
         <v>68</v>
       </c>
       <c r="B7" t="n">
-        <v>105.667282393624</v>
+        <v>105.667529242866</v>
       </c>
     </row>
     <row r="8">
@@ -1784,7 +1784,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="n">
-        <v>97.6199006514078</v>
+        <v>97.6200104539336</v>
       </c>
     </row>
     <row r="9">
@@ -1792,7 +1792,7 @@
         <v>70</v>
       </c>
       <c r="B9" t="n">
-        <v>78.7988598696828</v>
+        <v>78.798971822456</v>
       </c>
     </row>
     <row r="10">
@@ -1800,7 +1800,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="n">
-        <v>55.7454963786974</v>
+        <v>55.7456044405191</v>
       </c>
     </row>
     <row r="11">
@@ -1808,7 +1808,7 @@
         <v>72</v>
       </c>
       <c r="B11" t="n">
-        <v>53.7841023812626</v>
+        <v>53.7842084317809</v>
       </c>
     </row>
     <row r="12">
@@ -1816,7 +1816,7 @@
         <v>73</v>
       </c>
       <c r="B12" t="n">
-        <v>53.0237787594167</v>
+        <v>53.0238939413859</v>
       </c>
     </row>
     <row r="13">
@@ -1824,7 +1824,7 @@
         <v>74</v>
       </c>
       <c r="B13" t="n">
-        <v>49.9773448998184</v>
+        <v>49.9774545700953</v>
       </c>
     </row>
     <row r="14">
@@ -1832,7 +1832,7 @@
         <v>75</v>
       </c>
       <c r="B14" t="n">
-        <v>48.0733840887908</v>
+        <v>48.0727597037359</v>
       </c>
     </row>
     <row r="15">
@@ -1840,7 +1840,7 @@
         <v>76</v>
       </c>
       <c r="B15" t="n">
-        <v>45.2789704549205</v>
+        <v>45.2786410257155</v>
       </c>
     </row>
     <row r="16">
@@ -1848,7 +1848,7 @@
         <v>77</v>
       </c>
       <c r="B16" t="n">
-        <v>41.8999720082676</v>
+        <v>41.8994587062686</v>
       </c>
     </row>
     <row r="17">
@@ -1856,7 +1856,7 @@
         <v>78</v>
       </c>
       <c r="B17" t="n">
-        <v>38.0532599610642</v>
+        <v>38.0533745827657</v>
       </c>
     </row>
     <row r="18">
@@ -1864,7 +1864,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="n">
-        <v>34.8664284104069</v>
+        <v>34.8665486440876</v>
       </c>
     </row>
     <row r="19">
@@ -1872,7 +1872,7 @@
         <v>80</v>
       </c>
       <c r="B19" t="n">
-        <v>30.234305166861</v>
+        <v>30.2344224071871</v>
       </c>
     </row>
     <row r="20">
@@ -1880,7 +1880,7 @@
         <v>81</v>
       </c>
       <c r="B20" t="n">
-        <v>29.6066873425915</v>
+        <v>29.6038882125588</v>
       </c>
     </row>
     <row r="21">
@@ -1888,7 +1888,7 @@
         <v>82</v>
       </c>
       <c r="B21" t="n">
-        <v>29.2993238506721</v>
+        <v>29.2939327313113</v>
       </c>
     </row>
     <row r="22">
@@ -1896,7 +1896,7 @@
         <v>83</v>
       </c>
       <c r="B22" t="n">
-        <v>26.9337652237158</v>
+        <v>26.9338847737071</v>
       </c>
     </row>
     <row r="23">
@@ -1904,7 +1904,7 @@
         <v>84</v>
       </c>
       <c r="B23" t="n">
-        <v>26.3714106150685</v>
+        <v>26.3715335725925</v>
       </c>
     </row>
     <row r="24">
@@ -1912,7 +1912,7 @@
         <v>85</v>
       </c>
       <c r="B24" t="n">
-        <v>25.4163343786028</v>
+        <v>25.4161289330398</v>
       </c>
     </row>
     <row r="25">
@@ -1920,7 +1920,7 @@
         <v>86</v>
       </c>
       <c r="B25" t="n">
-        <v>25.1619658001022</v>
+        <v>25.1619773396717</v>
       </c>
     </row>
     <row r="26">
@@ -1928,7 +1928,7 @@
         <v>87</v>
       </c>
       <c r="B26" t="n">
-        <v>25.0986161976676</v>
+        <v>25.0987406676793</v>
       </c>
     </row>
     <row r="27">
@@ -1936,7 +1936,7 @@
         <v>88</v>
       </c>
       <c r="B27" t="n">
-        <v>20.8822354527917</v>
+        <v>20.8823438546053</v>
       </c>
     </row>
     <row r="28">
@@ -1944,7 +1944,7 @@
         <v>89</v>
       </c>
       <c r="B28" t="n">
-        <v>18.7934920304583</v>
+        <v>18.7936117730643</v>
       </c>
     </row>
     <row r="29">
@@ -1952,7 +1952,7 @@
         <v>90</v>
       </c>
       <c r="B29" t="n">
-        <v>17.5593323791082</v>
+        <v>17.555763872665</v>
       </c>
     </row>
     <row r="30">
@@ -1960,7 +1960,7 @@
         <v>91</v>
       </c>
       <c r="B30" t="n">
-        <v>15.8567984835836</v>
+        <v>15.8569053401172</v>
       </c>
     </row>
     <row r="31">
@@ -1968,7 +1968,7 @@
         <v>92</v>
       </c>
       <c r="B31" t="n">
-        <v>15.5358012274298</v>
+        <v>15.5359179212636</v>
       </c>
     </row>
     <row r="32">
@@ -1976,7 +1976,7 @@
         <v>93</v>
       </c>
       <c r="B32" t="n">
-        <v>15.1963119207898</v>
+        <v>15.1964280531625</v>
       </c>
     </row>
     <row r="33">
@@ -1984,7 +1984,7 @@
         <v>94</v>
       </c>
       <c r="B33" t="n">
-        <v>15.0200887756042</v>
+        <v>15.020205034054</v>
       </c>
     </row>
     <row r="34">
@@ -1992,7 +1992,7 @@
         <v>95</v>
       </c>
       <c r="B34" t="n">
-        <v>13.4759318348703</v>
+        <v>13.476152523452</v>
       </c>
     </row>
     <row r="35">
@@ -2000,7 +2000,7 @@
         <v>96</v>
       </c>
       <c r="B35" t="n">
-        <v>13.2211166796745</v>
+        <v>13.2212228253832</v>
       </c>
     </row>
     <row r="36">
@@ -2008,7 +2008,7 @@
         <v>97</v>
       </c>
       <c r="B36" t="n">
-        <v>12.5716357936045</v>
+        <v>12.5717697101014</v>
       </c>
     </row>
     <row r="37">
@@ -2016,7 +2016,7 @@
         <v>98</v>
       </c>
       <c r="B37" t="n">
-        <v>12.5237413069436</v>
+        <v>12.5238612856267</v>
       </c>
     </row>
     <row r="38">
@@ -2024,7 +2024,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="n">
-        <v>12.4544296675044</v>
+        <v>12.4544481869202</v>
       </c>
     </row>
     <row r="39">
@@ -2032,7 +2032,7 @@
         <v>100</v>
       </c>
       <c r="B39" t="n">
-        <v>12.0440957788722</v>
+        <v>12.0438017334375</v>
       </c>
     </row>
     <row r="40">
@@ -2040,7 +2040,7 @@
         <v>101</v>
       </c>
       <c r="B40" t="n">
-        <v>9.90312451374928</v>
+        <v>9.90290757740704</v>
       </c>
     </row>
     <row r="41">
@@ -2048,7 +2048,7 @@
         <v>102</v>
       </c>
       <c r="B41" t="n">
-        <v>9.81270657274646</v>
+        <v>9.81263042818695</v>
       </c>
     </row>
     <row r="42">
@@ -2056,7 +2056,7 @@
         <v>103</v>
       </c>
       <c r="B42" t="n">
-        <v>9.15973801366173</v>
+        <v>9.15985513828874</v>
       </c>
     </row>
     <row r="43">
@@ -2064,7 +2064,7 @@
         <v>104</v>
       </c>
       <c r="B43" t="n">
-        <v>9.05799226955743</v>
+        <v>9.05811068615802</v>
       </c>
     </row>
     <row r="44">
@@ -2072,7 +2072,7 @@
         <v>105</v>
       </c>
       <c r="B44" t="n">
-        <v>8.3897913628308</v>
+        <v>8.38990215667245</v>
       </c>
     </row>
     <row r="45">
@@ -2080,7 +2080,7 @@
         <v>106</v>
       </c>
       <c r="B45" t="n">
-        <v>6.63340704529754</v>
+        <v>6.63319041477624</v>
       </c>
     </row>
     <row r="46">
@@ -2088,7 +2088,7 @@
         <v>107</v>
       </c>
       <c r="B46" t="n">
-        <v>6.5133035037067</v>
+        <v>6.51341988172355</v>
       </c>
     </row>
     <row r="47">
@@ -2096,7 +2096,7 @@
         <v>108</v>
       </c>
       <c r="B47" t="n">
-        <v>6.48684021606382</v>
+        <v>6.48696150471856</v>
       </c>
     </row>
     <row r="48">
@@ -2104,7 +2104,7 @@
         <v>109</v>
       </c>
       <c r="B48" t="n">
-        <v>5.94383624969695</v>
+        <v>5.94395272761954</v>
       </c>
     </row>
     <row r="49">
@@ -2112,7 +2112,7 @@
         <v>110</v>
       </c>
       <c r="B49" t="n">
-        <v>5.04979463791619</v>
+        <v>5.04989597237642</v>
       </c>
     </row>
     <row r="50">
@@ -2120,7 +2120,7 @@
         <v>111</v>
       </c>
       <c r="B50" t="n">
-        <v>4.99303261565805</v>
+        <v>4.99176109995655</v>
       </c>
     </row>
     <row r="51">
@@ -2128,7 +2128,7 @@
         <v>112</v>
       </c>
       <c r="B51" t="n">
-        <v>4.80263086461322</v>
+        <v>4.80274794643</v>
       </c>
     </row>
     <row r="52">
@@ -2136,7 +2136,7 @@
         <v>113</v>
       </c>
       <c r="B52" t="n">
-        <v>4.73817634497588</v>
+        <v>4.73696353951607</v>
       </c>
     </row>
     <row r="53">
@@ -2144,7 +2144,7 @@
         <v>114</v>
       </c>
       <c r="B53" t="n">
-        <v>4.32297849409216</v>
+        <v>4.32311482209655</v>
       </c>
     </row>
     <row r="54">
@@ -2152,7 +2152,7 @@
         <v>115</v>
       </c>
       <c r="B54" t="n">
-        <v>4.26904802666119</v>
+        <v>4.26916433308626</v>
       </c>
     </row>
     <row r="55">
@@ -2160,7 +2160,7 @@
         <v>116</v>
       </c>
       <c r="B55" t="n">
-        <v>3.99872046248461</v>
+        <v>3.99884006368276</v>
       </c>
     </row>
     <row r="56">
@@ -2168,7 +2168,7 @@
         <v>117</v>
       </c>
       <c r="B56" t="n">
-        <v>3.91640736388767</v>
+        <v>3.91610551675662</v>
       </c>
     </row>
     <row r="57">
@@ -2176,7 +2176,7 @@
         <v>118</v>
       </c>
       <c r="B57" t="n">
-        <v>3.81248608182475</v>
+        <v>3.81235703596084</v>
       </c>
     </row>
     <row r="58">
@@ -2184,7 +2184,7 @@
         <v>119</v>
       </c>
       <c r="B58" t="n">
-        <v>3.66979451563877</v>
+        <v>3.66965056921662</v>
       </c>
     </row>
     <row r="59">
@@ -2192,7 +2192,7 @@
         <v>120</v>
       </c>
       <c r="B59" t="n">
-        <v>3.6279573246119</v>
+        <v>3.62807467954036</v>
       </c>
     </row>
     <row r="60">
@@ -2200,7 +2200,7 @@
         <v>121</v>
       </c>
       <c r="B60" t="n">
-        <v>3.22351621291509</v>
+        <v>3.22363182843953</v>
       </c>
     </row>
     <row r="61">
@@ -2208,7 +2208,7 @@
         <v>122</v>
       </c>
       <c r="B61" t="n">
-        <v>3.0749728128745</v>
+        <v>3.07324312415748</v>
       </c>
     </row>
     <row r="62">
@@ -2216,7 +2216,7 @@
         <v>123</v>
       </c>
       <c r="B62" t="n">
-        <v>2.96095501518306</v>
+        <v>2.96040219885768</v>
       </c>
     </row>
     <row r="63">
@@ -2224,7 +2224,7 @@
         <v>124</v>
       </c>
       <c r="B63" t="n">
-        <v>2.80952598598794</v>
+        <v>2.8096439814303</v>
       </c>
     </row>
     <row r="64">
@@ -2232,7 +2232,7 @@
         <v>125</v>
       </c>
       <c r="B64" t="n">
-        <v>2.59349057121388</v>
+        <v>2.59361017955284</v>
       </c>
     </row>
     <row r="65">
@@ -2240,7 +2240,7 @@
         <v>126</v>
       </c>
       <c r="B65" t="n">
-        <v>2.51850255171226</v>
+        <v>2.51873849961158</v>
       </c>
     </row>
     <row r="66">
@@ -2256,7 +2256,7 @@
         <v>128</v>
       </c>
       <c r="B67" t="n">
-        <v>2.34140272054471</v>
+        <v>2.34127873758682</v>
       </c>
     </row>
     <row r="68">
@@ -2264,7 +2264,7 @@
         <v>129</v>
       </c>
       <c r="B68" t="n">
-        <v>2.07326875306419</v>
+        <v>2.07338761967411</v>
       </c>
     </row>
     <row r="69">
@@ -2272,7 +2272,7 @@
         <v>130</v>
       </c>
       <c r="B69" t="n">
-        <v>2.05693127227206</v>
+        <v>2.05689350028882</v>
       </c>
     </row>
     <row r="70">
@@ -2280,7 +2280,7 @@
         <v>131</v>
       </c>
       <c r="B70" t="n">
-        <v>1.86172924574933</v>
+        <v>1.86184679909448</v>
       </c>
     </row>
     <row r="71">
@@ -2288,7 +2288,7 @@
         <v>132</v>
       </c>
       <c r="B71" t="n">
-        <v>1.83712407054604</v>
+        <v>1.83724196988251</v>
       </c>
     </row>
     <row r="72">
@@ -2296,7 +2296,7 @@
         <v>133</v>
       </c>
       <c r="B72" t="n">
-        <v>1.83575558785628</v>
+        <v>1.83586488260237</v>
       </c>
     </row>
     <row r="73">
@@ -2304,7 +2304,7 @@
         <v>134</v>
       </c>
       <c r="B73" t="n">
-        <v>1.66820988508381</v>
+        <v>1.66832756978321</v>
       </c>
     </row>
     <row r="74">
@@ -2312,7 +2312,7 @@
         <v>135</v>
       </c>
       <c r="B74" t="n">
-        <v>1.41509162685255</v>
+        <v>1.41520913284778</v>
       </c>
     </row>
     <row r="75">
@@ -2320,7 +2320,7 @@
         <v>136</v>
       </c>
       <c r="B75" t="n">
-        <v>1.39156556135639</v>
+        <v>1.39155482413541</v>
       </c>
     </row>
     <row r="76">
@@ -2328,7 +2328,7 @@
         <v>137</v>
       </c>
       <c r="B76" t="n">
-        <v>1.37872824356557</v>
+        <v>1.3784150274351</v>
       </c>
     </row>
     <row r="77">
@@ -2336,7 +2336,7 @@
         <v>138</v>
       </c>
       <c r="B77" t="n">
-        <v>1.37104674636937</v>
+        <v>1.35606697347091</v>
       </c>
     </row>
     <row r="78">
@@ -2344,7 +2344,7 @@
         <v>139</v>
       </c>
       <c r="B78" t="n">
-        <v>1.34622640447513</v>
+        <v>1.34634345910685</v>
       </c>
     </row>
     <row r="79">
@@ -2352,7 +2352,7 @@
         <v>140</v>
       </c>
       <c r="B79" t="n">
-        <v>1.27303460939237</v>
+        <v>1.27315319189474</v>
       </c>
     </row>
     <row r="80">
@@ -2360,7 +2360,7 @@
         <v>141</v>
       </c>
       <c r="B80" t="n">
-        <v>1.1943474457193</v>
+        <v>1.19446488027903</v>
       </c>
     </row>
     <row r="81">
@@ -2368,7 +2368,7 @@
         <v>142</v>
       </c>
       <c r="B81" t="n">
-        <v>1.17904259157617</v>
+        <v>1.17916048184456</v>
       </c>
     </row>
     <row r="82">
@@ -2376,7 +2376,7 @@
         <v>143</v>
       </c>
       <c r="B82" t="n">
-        <v>1.13346307372864</v>
+        <v>1.13327011953983</v>
       </c>
     </row>
     <row r="83">
@@ -2384,7 +2384,7 @@
         <v>144</v>
       </c>
       <c r="B83" t="n">
-        <v>1.10594488496462</v>
+        <v>1.10571181128032</v>
       </c>
     </row>
     <row r="84">
@@ -2392,7 +2392,7 @@
         <v>145</v>
       </c>
       <c r="B84" t="n">
-        <v>1.09034181477187</v>
+        <v>1.08953469264216</v>
       </c>
     </row>
     <row r="85">
@@ -2400,7 +2400,7 @@
         <v>146</v>
       </c>
       <c r="B85" t="n">
-        <v>1.08705592140544</v>
+        <v>1.08682764725851</v>
       </c>
     </row>
     <row r="86">
@@ -2408,7 +2408,7 @@
         <v>147</v>
       </c>
       <c r="B86" t="n">
-        <v>1.04141277147744</v>
+        <v>1.04153032342991</v>
       </c>
     </row>
     <row r="87">
@@ -2416,7 +2416,7 @@
         <v>148</v>
       </c>
       <c r="B87" t="n">
-        <v>1.03261958841435</v>
+        <v>1.03284150993919</v>
       </c>
     </row>
     <row r="88">
@@ -2424,7 +2424,7 @@
         <v>149</v>
       </c>
       <c r="B88" t="n">
-        <v>0.867895856308705</v>
+        <v>0.868013935698825</v>
       </c>
     </row>
     <row r="89">
@@ -2432,7 +2432,7 @@
         <v>150</v>
       </c>
       <c r="B89" t="n">
-        <v>0.861484337643331</v>
+        <v>0.861601987977717</v>
       </c>
     </row>
     <row r="90">
@@ -2440,7 +2440,7 @@
         <v>151</v>
       </c>
       <c r="B90" t="n">
-        <v>0.824227516575347</v>
+        <v>0.824345076580402</v>
       </c>
     </row>
     <row r="91">
@@ -2448,7 +2448,7 @@
         <v>152</v>
       </c>
       <c r="B91" t="n">
-        <v>0.803763861237097</v>
+        <v>0.803880776853297</v>
       </c>
     </row>
     <row r="92">
@@ -2456,7 +2456,7 @@
         <v>153</v>
       </c>
       <c r="B92" t="n">
-        <v>0.775470138897721</v>
+        <v>0.774860593054094</v>
       </c>
     </row>
     <row r="93">
@@ -2464,7 +2464,7 @@
         <v>154</v>
       </c>
       <c r="B93" t="n">
-        <v>0.752349479454739</v>
+        <v>0.752467053014986</v>
       </c>
     </row>
     <row r="94">
@@ -2472,7 +2472,7 @@
         <v>155</v>
       </c>
       <c r="B94" t="n">
-        <v>0.742292401670528</v>
+        <v>0.742409999877089</v>
       </c>
     </row>
     <row r="95">
@@ -2480,7 +2480,7 @@
         <v>156</v>
       </c>
       <c r="B95" t="n">
-        <v>0.716918638711232</v>
+        <v>0.71703601968462</v>
       </c>
     </row>
     <row r="96">
@@ -2488,7 +2488,7 @@
         <v>157</v>
       </c>
       <c r="B96" t="n">
-        <v>0.710354996528178</v>
+        <v>0.710472623526309</v>
       </c>
     </row>
     <row r="97">
@@ -2496,7 +2496,7 @@
         <v>158</v>
       </c>
       <c r="B97" t="n">
-        <v>0.704653655431748</v>
+        <v>0.704770691726492</v>
       </c>
     </row>
     <row r="98">
@@ -2504,7 +2504,7 @@
         <v>159</v>
       </c>
       <c r="B98" t="n">
-        <v>0.681177109908324</v>
+        <v>0.681294888289127</v>
       </c>
     </row>
     <row r="99">
@@ -2512,7 +2512,7 @@
         <v>160</v>
       </c>
       <c r="B99" t="n">
-        <v>0.673693552091918</v>
+        <v>0.673811119182354</v>
       </c>
     </row>
     <row r="100">
@@ -2520,7 +2520,7 @@
         <v>161</v>
       </c>
       <c r="B100" t="n">
-        <v>0.664476824648182</v>
+        <v>0.66459419029735</v>
       </c>
     </row>
     <row r="101">
@@ -2528,7 +2528,7 @@
         <v>162</v>
       </c>
       <c r="B101" t="n">
-        <v>0.657135099107899</v>
+        <v>0.657252402937339</v>
       </c>
     </row>
     <row r="102">
@@ -2536,7 +2536,7 @@
         <v>163</v>
       </c>
       <c r="B102" t="n">
-        <v>0.633100986097252</v>
+        <v>0.63321858035688</v>
       </c>
     </row>
     <row r="103">
@@ -2544,7 +2544,7 @@
         <v>164</v>
       </c>
       <c r="B103" t="n">
-        <v>0.628737885487038</v>
+        <v>0.628753333370248</v>
       </c>
     </row>
     <row r="104">
@@ -2552,7 +2552,7 @@
         <v>165</v>
       </c>
       <c r="B104" t="n">
-        <v>0.627439099584635</v>
+        <v>0.627558497305675</v>
       </c>
     </row>
     <row r="105">
@@ -2560,7 +2560,7 @@
         <v>166</v>
       </c>
       <c r="B105" t="n">
-        <v>0.618016070913641</v>
+        <v>0.618133110491617</v>
       </c>
     </row>
     <row r="106">
@@ -2568,7 +2568,7 @@
         <v>28</v>
       </c>
       <c r="B106" t="n">
-        <v>0.593195693864616</v>
+        <v>0.585643464200109</v>
       </c>
     </row>
     <row r="107">
@@ -2576,7 +2576,7 @@
         <v>167</v>
       </c>
       <c r="B107" t="n">
-        <v>0.581423138756837</v>
+        <v>0.581536800851818</v>
       </c>
     </row>
     <row r="108">
@@ -2584,7 +2584,7 @@
         <v>168</v>
       </c>
       <c r="B108" t="n">
-        <v>0.578585718250423</v>
+        <v>0.578703355774493</v>
       </c>
     </row>
     <row r="109">
@@ -2592,7 +2592,7 @@
         <v>169</v>
       </c>
       <c r="B109" t="n">
-        <v>0.570057045720286</v>
+        <v>0.570174647065111</v>
       </c>
     </row>
     <row r="110">
@@ -2600,7 +2600,7 @@
         <v>170</v>
       </c>
       <c r="B110" t="n">
-        <v>0.544903180670939</v>
+        <v>0.545020589416799</v>
       </c>
     </row>
     <row r="111">
@@ -2608,7 +2608,7 @@
         <v>171</v>
       </c>
       <c r="B111" t="n">
-        <v>0.526828028371623</v>
+        <v>0.52694562975194</v>
       </c>
     </row>
     <row r="112">
@@ -2616,7 +2616,7 @@
         <v>172</v>
       </c>
       <c r="B112" t="n">
-        <v>0.509208342997091</v>
+        <v>0.509325837543411</v>
       </c>
     </row>
     <row r="113">
@@ -2624,7 +2624,7 @@
         <v>173</v>
       </c>
       <c r="B113" t="n">
-        <v>0.50459384676247</v>
+        <v>0.504710975409813</v>
       </c>
     </row>
     <row r="114">
@@ -2632,7 +2632,7 @@
         <v>174</v>
       </c>
       <c r="B114" t="n">
-        <v>0.501910274392442</v>
+        <v>0.501765856918293</v>
       </c>
     </row>
     <row r="115">
@@ -2640,7 +2640,7 @@
         <v>175</v>
       </c>
       <c r="B115" t="n">
-        <v>0.493005181480563</v>
+        <v>0.4931227913293</v>
       </c>
     </row>
     <row r="116">
@@ -2648,7 +2648,7 @@
         <v>176</v>
       </c>
       <c r="B116" t="n">
-        <v>0.477676107853913</v>
+        <v>0.477793626689722</v>
       </c>
     </row>
     <row r="117">
@@ -2656,7 +2656,7 @@
         <v>177</v>
       </c>
       <c r="B117" t="n">
-        <v>0.464483547942825</v>
+        <v>0.46463580657391</v>
       </c>
     </row>
     <row r="118">
@@ -2664,7 +2664,7 @@
         <v>178</v>
       </c>
       <c r="B118" t="n">
-        <v>0.460887677291465</v>
+        <v>0.461005351385604</v>
       </c>
     </row>
     <row r="119">
@@ -2672,7 +2672,7 @@
         <v>179</v>
       </c>
       <c r="B119" t="n">
-        <v>0.413690516066874</v>
+        <v>0.413807690194662</v>
       </c>
     </row>
     <row r="120">
@@ -2680,7 +2680,7 @@
         <v>180</v>
       </c>
       <c r="B120" t="n">
-        <v>0.394201895059809</v>
+        <v>0.394340848106566</v>
       </c>
     </row>
     <row r="121">
@@ -2688,7 +2688,7 @@
         <v>181</v>
       </c>
       <c r="B121" t="n">
-        <v>0.391897475298288</v>
+        <v>0.392053177830799</v>
       </c>
     </row>
     <row r="122">
@@ -2696,7 +2696,7 @@
         <v>182</v>
       </c>
       <c r="B122" t="n">
-        <v>0.386890547784881</v>
+        <v>0.387029537840346</v>
       </c>
     </row>
     <row r="123">
@@ -2704,7 +2704,7 @@
         <v>183</v>
       </c>
       <c r="B123" t="n">
-        <v>0.382419182882089</v>
+        <v>0.381959735153278</v>
       </c>
     </row>
     <row r="124">
@@ -2712,7 +2712,7 @@
         <v>184</v>
       </c>
       <c r="B124" t="n">
-        <v>0.381386061613438</v>
+        <v>0.379427229333532</v>
       </c>
     </row>
     <row r="125">
@@ -2720,7 +2720,7 @@
         <v>185</v>
       </c>
       <c r="B125" t="n">
-        <v>0.379309621671865</v>
+        <v>0.377635822930571</v>
       </c>
     </row>
     <row r="126">
@@ -2728,7 +2728,7 @@
         <v>186</v>
       </c>
       <c r="B126" t="n">
-        <v>0.373012705256503</v>
+        <v>0.370354416557028</v>
       </c>
     </row>
     <row r="127">
@@ -2736,7 +2736,7 @@
         <v>187</v>
       </c>
       <c r="B127" t="n">
-        <v>0.370215416178614</v>
+        <v>0.370025301985331</v>
       </c>
     </row>
     <row r="128">
@@ -2744,7 +2744,7 @@
         <v>188</v>
       </c>
       <c r="B128" t="n">
-        <v>0.370035654249857</v>
+        <v>0.369082276870947</v>
       </c>
     </row>
     <row r="129">
@@ -2752,7 +2752,7 @@
         <v>189</v>
       </c>
       <c r="B129" t="n">
-        <v>0.366692319561139</v>
+        <v>0.366831310003451</v>
       </c>
     </row>
     <row r="130">
@@ -2760,7 +2760,7 @@
         <v>190</v>
       </c>
       <c r="B130" t="n">
-        <v>0.359830767508358</v>
+        <v>0.359948377512569</v>
       </c>
     </row>
     <row r="131">
@@ -2768,7 +2768,7 @@
         <v>191</v>
       </c>
       <c r="B131" t="n">
-        <v>0.358462907721728</v>
+        <v>0.358554372714931</v>
       </c>
     </row>
     <row r="132">
@@ -2776,7 +2776,7 @@
         <v>192</v>
       </c>
       <c r="B132" t="n">
-        <v>0.354833164499855</v>
+        <v>0.351897154133667</v>
       </c>
     </row>
     <row r="133">
@@ -2784,7 +2784,7 @@
         <v>193</v>
       </c>
       <c r="B133" t="n">
-        <v>0.351758163617146</v>
+        <v>0.351879598242447</v>
       </c>
     </row>
     <row r="134">
@@ -2792,7 +2792,7 @@
         <v>194</v>
       </c>
       <c r="B134" t="n">
-        <v>0.351740607731796</v>
+        <v>0.351814238433637</v>
       </c>
     </row>
     <row r="135">
@@ -2800,7 +2800,7 @@
         <v>195</v>
       </c>
       <c r="B135" t="n">
-        <v>0.351675247853753</v>
+        <v>0.351775871853511</v>
       </c>
     </row>
     <row r="136">
@@ -2808,7 +2808,7 @@
         <v>196</v>
       </c>
       <c r="B136" t="n">
-        <v>0.351637087915529</v>
+        <v>0.351682359548034</v>
       </c>
     </row>
     <row r="137">
@@ -2816,7 +2816,7 @@
         <v>197</v>
       </c>
       <c r="B137" t="n">
-        <v>0.351590894405607</v>
+        <v>0.351529405188472</v>
       </c>
     </row>
     <row r="138">
@@ -2824,7 +2824,7 @@
         <v>198</v>
       </c>
       <c r="B138" t="n">
-        <v>0.351390415087983</v>
+        <v>0.351460692007772</v>
       </c>
     </row>
     <row r="139">
@@ -2832,7 +2832,7 @@
         <v>199</v>
       </c>
       <c r="B139" t="n">
-        <v>0.351321701153311</v>
+        <v>0.351363150985716</v>
       </c>
     </row>
     <row r="140">
@@ -2840,7 +2840,7 @@
         <v>200</v>
       </c>
       <c r="B140" t="n">
-        <v>0.351224159355696</v>
+        <v>0.351363150284967</v>
       </c>
     </row>
     <row r="141">
@@ -2848,7 +2848,7 @@
         <v>201</v>
       </c>
       <c r="B141" t="n">
-        <v>0.351224158877173</v>
+        <v>0.351363149806233</v>
       </c>
     </row>
     <row r="142">
@@ -2856,7 +2856,7 @@
         <v>202</v>
       </c>
       <c r="B142" t="n">
-        <v>0.351224158711744</v>
+        <v>0.351363149640497</v>
       </c>
     </row>
     <row r="143">
@@ -2864,7 +2864,7 @@
         <v>203</v>
       </c>
       <c r="B143" t="n">
-        <v>0.351224158582765</v>
+        <v>0.351363149511382</v>
       </c>
     </row>
     <row r="144">
@@ -2872,7 +2872,7 @@
         <v>204</v>
       </c>
       <c r="B144" t="n">
-        <v>0.351224158582752</v>
+        <v>0.351363149511354</v>
       </c>
     </row>
     <row r="145">
@@ -2880,7 +2880,7 @@
         <v>205</v>
       </c>
       <c r="B145" t="n">
-        <v>0.351192336062621</v>
+        <v>0.351331326813973</v>
       </c>
     </row>
     <row r="146">
@@ -2888,7 +2888,7 @@
         <v>206</v>
       </c>
       <c r="B146" t="n">
-        <v>0.351167498201752</v>
+        <v>0.351306487194202</v>
       </c>
     </row>
     <row r="147">
@@ -2896,7 +2896,7 @@
         <v>30</v>
       </c>
       <c r="B147" t="n">
-        <v>0.351147455997059</v>
+        <v>0.351286430683572</v>
       </c>
     </row>
     <row r="148">
@@ -2904,7 +2904,7 @@
         <v>207</v>
       </c>
       <c r="B148" t="n">
-        <v>0.351121651112203</v>
+        <v>0.351260641468633</v>
       </c>
     </row>
     <row r="149">
@@ -2912,7 +2912,7 @@
         <v>208</v>
       </c>
       <c r="B149" t="n">
-        <v>0.351113083323579</v>
+        <v>0.351252073632187</v>
       </c>
     </row>
     <row r="150">
@@ -2920,7 +2920,7 @@
         <v>209</v>
       </c>
       <c r="B150" t="n">
-        <v>0.350991096919047</v>
+        <v>0.351130038495845</v>
       </c>
     </row>
     <row r="151">
@@ -2928,7 +2928,7 @@
         <v>210</v>
       </c>
       <c r="B151" t="n">
-        <v>0.350929358249242</v>
+        <v>0.351068286752965</v>
       </c>
     </row>
     <row r="152">
@@ -2936,7 +2936,7 @@
         <v>211</v>
       </c>
       <c r="B152" t="n">
-        <v>0.350882648588827</v>
+        <v>0.351021567200955</v>
       </c>
     </row>
     <row r="153">
@@ -2944,7 +2944,7 @@
         <v>212</v>
       </c>
       <c r="B153" t="n">
-        <v>0.350508619763976</v>
+        <v>0.350668282383311</v>
       </c>
     </row>
     <row r="154">
@@ -2952,7 +2952,7 @@
         <v>33</v>
       </c>
       <c r="B154" t="n">
-        <v>0.350340180395379</v>
+        <v>0.350479166389934</v>
       </c>
     </row>
     <row r="155">
@@ -2960,7 +2960,7 @@
         <v>213</v>
       </c>
       <c r="B155" t="n">
-        <v>0.347923120396244</v>
+        <v>0.348061408312438</v>
       </c>
     </row>
     <row r="156">
@@ -2968,7 +2968,7 @@
         <v>214</v>
       </c>
       <c r="B156" t="n">
-        <v>0.346056469966773</v>
+        <v>0.346194378988225</v>
       </c>
     </row>
     <row r="157">
@@ -2976,7 +2976,7 @@
         <v>215</v>
       </c>
       <c r="B157" t="n">
-        <v>0.0791793371196524</v>
+        <v>0.0793168096193734</v>
       </c>
     </row>
   </sheetData>
@@ -3019,13 +3019,13 @@
         <v>140</v>
       </c>
       <c r="C2" t="n">
-        <v>0.470173609392365</v>
+        <v>0.470292191894741</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>5.87170108996351</v>
+        <v>5.8718233657334</v>
       </c>
     </row>
     <row r="3">
@@ -3033,16 +3033,16 @@
         <v>2023</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C3" t="n">
-        <v>0.351758163617146</v>
+        <v>0.351897154133667</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>5.75263114515787</v>
+        <v>5.75275247385177</v>
       </c>
     </row>
     <row r="4">
@@ -3053,13 +3053,13 @@
         <v>126</v>
       </c>
       <c r="C4" t="n">
-        <v>1.42903655171226</v>
+        <v>1.42927249961158</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>12.232269986505</v>
+        <v>12.2325133471782</v>
       </c>
     </row>
     <row r="5">
@@ -3070,13 +3070,13 @@
         <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>0.458325516575347</v>
+        <v>0.458443076580402</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>5.8599331157288</v>
+        <v>5.86005438973344</v>
       </c>
     </row>
     <row r="6">
@@ -3087,13 +3087,13 @@
         <v>99</v>
       </c>
       <c r="C6" t="n">
-        <v>5.51249866750437</v>
+        <v>5.51251718692018</v>
       </c>
       <c r="D6" t="n">
-        <v>0.229341340266983</v>
+        <v>0.229428874483924</v>
       </c>
       <c r="E6" t="n">
-        <v>10.9183128279376</v>
+        <v>10.9183349318508</v>
       </c>
     </row>
     <row r="7">
@@ -3104,13 +3104,13 @@
         <v>159</v>
       </c>
       <c r="C7" t="n">
-        <v>0.388719109908324</v>
+        <v>0.388836888289127</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>5.79029668161912</v>
+        <v>5.79041816909692</v>
       </c>
     </row>
     <row r="8">
@@ -3121,13 +3121,13 @@
         <v>166</v>
       </c>
       <c r="C8" t="n">
-        <v>0.618016070913641</v>
+        <v>0.618133110491617</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>6.01978808970967</v>
+        <v>6.01990884351696</v>
       </c>
     </row>
     <row r="9">
@@ -3138,13 +3138,13 @@
         <v>95</v>
       </c>
       <c r="C9" t="n">
-        <v>3.14525083487029</v>
+        <v>3.14547152345199</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0349954465899406</v>
+        <v>0.0352141597005494</v>
       </c>
       <c r="E9" t="n">
-        <v>8.87428122020188</v>
+        <v>8.87415853349451</v>
       </c>
     </row>
     <row r="10">
@@ -3155,13 +3155,13 @@
         <v>136</v>
       </c>
       <c r="C10" t="n">
-        <v>1.34821356135639</v>
+        <v>1.34820282413541</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>6.75008805447529</v>
+        <v>6.75008097820748</v>
       </c>
     </row>
     <row r="11">
@@ -3169,16 +3169,16 @@
         <v>2023</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C11" t="n">
-        <v>0.370035654249857</v>
+        <v>0.370025301985331</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>5.77163110007636</v>
+        <v>5.77162443911143</v>
       </c>
     </row>
     <row r="12">
@@ -3189,13 +3189,13 @@
         <v>124</v>
       </c>
       <c r="C12" t="n">
-        <v>0.605610985987938</v>
+        <v>0.6057289814303</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>6.00717693298387</v>
+        <v>6.0072986438056</v>
       </c>
     </row>
     <row r="13">
@@ -3206,13 +3206,13 @@
         <v>135</v>
       </c>
       <c r="C13" t="n">
-        <v>0.443680626852554</v>
+        <v>0.443798132847784</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>5.84528544444127</v>
+        <v>5.84540666177982</v>
       </c>
     </row>
     <row r="14">
@@ -3223,13 +3223,13 @@
         <v>175</v>
       </c>
       <c r="C14" t="n">
-        <v>0.360031181480563</v>
+        <v>0.3601487913293</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>5.76162424437039</v>
+        <v>5.76174556614329</v>
       </c>
     </row>
     <row r="15">
@@ -3240,13 +3240,13 @@
         <v>132</v>
       </c>
       <c r="C15" t="n">
-        <v>0.519506070546042</v>
+        <v>0.519623969882507</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>5.92107724919565</v>
+        <v>5.92119886258119</v>
       </c>
     </row>
     <row r="16">
@@ -3257,13 +3257,13 @@
         <v>82</v>
       </c>
       <c r="C16" t="n">
-        <v>4.04251185067205</v>
+        <v>4.04053073131132</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>9.44552687461774</v>
+        <v>9.44354874888737</v>
       </c>
     </row>
     <row r="17">
@@ -3274,13 +3274,13 @@
         <v>70</v>
       </c>
       <c r="C17" t="n">
-        <v>7.13073886968275</v>
+        <v>7.13085082245599</v>
       </c>
       <c r="D17" t="n">
-        <v>1.72591891580601</v>
+        <v>1.72602717602809</v>
       </c>
       <c r="E17" t="n">
-        <v>12.5355588235595</v>
+        <v>12.5356744688839</v>
       </c>
     </row>
     <row r="18">
@@ -3291,13 +3291,13 @@
         <v>160</v>
       </c>
       <c r="C18" t="n">
-        <v>0.420284552091918</v>
+        <v>0.420402119182354</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>5.8218859337351</v>
+        <v>5.8220072125124</v>
       </c>
     </row>
     <row r="19">
@@ -3308,13 +3308,13 @@
         <v>208</v>
       </c>
       <c r="C19" t="n">
-        <v>0.351113083323579</v>
+        <v>0.351252073632187</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>5.7513410679769</v>
+        <v>5.75146239625702</v>
       </c>
     </row>
     <row r="20">
@@ -3325,13 +3325,13 @@
         <v>72</v>
       </c>
       <c r="C20" t="n">
-        <v>5.31258338126261</v>
+        <v>5.31268943178085</v>
       </c>
       <c r="D20" t="n">
-        <v>0.106574374162388</v>
+        <v>0.106705574820918</v>
       </c>
       <c r="E20" t="n">
-        <v>10.718335651844</v>
+        <v>10.7184454300305</v>
       </c>
     </row>
     <row r="21">
@@ -3342,13 +3342,13 @@
         <v>138</v>
       </c>
       <c r="C21" t="n">
-        <v>0.283664746369367</v>
+        <v>0.282651973470907</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>5.73565834412987</v>
+        <v>5.73464934512539</v>
       </c>
     </row>
     <row r="22">
@@ -3359,13 +3359,13 @@
         <v>213</v>
       </c>
       <c r="C22" t="n">
-        <v>0.347923120396244</v>
+        <v>0.348061408312438</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>5.74498183872479</v>
+        <v>5.74510176200942</v>
       </c>
     </row>
     <row r="23">
@@ -3376,13 +3376,13 @@
         <v>86</v>
       </c>
       <c r="C23" t="n">
-        <v>2.26418480010224</v>
+        <v>2.26419633967174</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>7.66589048570069</v>
+        <v>7.6659056774552</v>
       </c>
     </row>
     <row r="24">
@@ -3393,13 +3393,13 @@
         <v>200</v>
       </c>
       <c r="C24" t="n">
-        <v>0.351224159355696</v>
+        <v>0.351363150284967</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>5.75156297074125</v>
+        <v>5.75168430025742</v>
       </c>
     </row>
     <row r="25">
@@ -3410,13 +3410,13 @@
         <v>30</v>
       </c>
       <c r="C25" t="n">
-        <v>0.351147455997059</v>
+        <v>0.351286430683572</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>5.75140995898754</v>
+        <v>5.75153125601313</v>
       </c>
     </row>
     <row r="26">
@@ -3427,13 +3427,13 @@
         <v>153</v>
       </c>
       <c r="C26" t="n">
-        <v>0.775470138897721</v>
+        <v>0.774860593054094</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>6.19430452049604</v>
+        <v>6.19369853446414</v>
       </c>
     </row>
     <row r="27">
@@ -3444,13 +3444,13 @@
         <v>149</v>
       </c>
       <c r="C27" t="n">
-        <v>0.647411856308705</v>
+        <v>0.647529935698825</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>6.04913312121948</v>
+        <v>6.04925491455786</v>
       </c>
     </row>
     <row r="28">
@@ -3461,13 +3461,13 @@
         <v>137</v>
       </c>
       <c r="C28" t="n">
-        <v>0.436996243565568</v>
+        <v>0.436683027435103</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>5.83857105309356</v>
+        <v>5.83826148197575</v>
       </c>
     </row>
     <row r="29">
@@ -3478,13 +3478,13 @@
         <v>129</v>
       </c>
       <c r="C29" t="n">
-        <v>0.538325753064191</v>
+        <v>0.538444619674109</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>5.93985348454031</v>
+        <v>5.93997604410691</v>
       </c>
     </row>
     <row r="30">
@@ -3495,13 +3495,13 @@
         <v>139</v>
       </c>
       <c r="C30" t="n">
-        <v>0.88427940447513</v>
+        <v>0.884396459106855</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>6.28604393257209</v>
+        <v>6.28616470136325</v>
       </c>
     </row>
     <row r="31">
@@ -3509,16 +3509,16 @@
         <v>2023</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C31" t="n">
-        <v>0.351321701153311</v>
+        <v>0.351460692007772</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>5.75175808459634</v>
+        <v>5.75187941396343</v>
       </c>
     </row>
     <row r="32">
@@ -3529,13 +3529,13 @@
         <v>145</v>
       </c>
       <c r="C32" t="n">
-        <v>0.408690814771866</v>
+        <v>0.407883692642157</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>5.8393993211353</v>
+        <v>5.83859582465007</v>
       </c>
     </row>
     <row r="33">
@@ -3546,13 +3546,13 @@
         <v>142</v>
       </c>
       <c r="C33" t="n">
-        <v>0.456334591576169</v>
+        <v>0.456452481844564</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>5.85793475892729</v>
+        <v>5.85805637519443</v>
       </c>
     </row>
     <row r="34">
@@ -3563,13 +3563,13 @@
         <v>91</v>
       </c>
       <c r="C34" t="n">
-        <v>14.2851884835836</v>
+        <v>14.2852953401172</v>
       </c>
       <c r="D34" t="n">
-        <v>8.85660984497127</v>
+        <v>8.8567129701711</v>
       </c>
       <c r="E34" t="n">
-        <v>19.7137671221958</v>
+        <v>19.7138777100633</v>
       </c>
     </row>
     <row r="35">
@@ -3580,13 +3580,13 @@
         <v>144</v>
       </c>
       <c r="C35" t="n">
-        <v>0.473310884964616</v>
+        <v>0.473077811280318</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>5.87492521197447</v>
+        <v>5.87469578465236</v>
       </c>
     </row>
     <row r="36">
@@ -3597,13 +3597,13 @@
         <v>146</v>
       </c>
       <c r="C36" t="n">
-        <v>0.487891921405442</v>
+        <v>0.487952647258509</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>5.88951138204399</v>
+        <v>5.88957584863854</v>
       </c>
     </row>
     <row r="37">
@@ -3614,13 +3614,13 @@
         <v>83</v>
       </c>
       <c r="C37" t="n">
-        <v>3.93013922371576</v>
+        <v>3.93025877370714</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>9.33620316438991</v>
+        <v>9.33632663180384</v>
       </c>
     </row>
     <row r="38">
@@ -3631,13 +3631,13 @@
         <v>104</v>
       </c>
       <c r="C38" t="n">
-        <v>1.14032826955743</v>
+        <v>1.14044668615802</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>6.54229521531609</v>
+        <v>6.54241740076341</v>
       </c>
     </row>
     <row r="39">
@@ -3648,13 +3648,13 @@
         <v>143</v>
       </c>
       <c r="C39" t="n">
-        <v>0.487676073728638</v>
+        <v>0.487483119539831</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>5.88922539042071</v>
+        <v>5.88903610560283</v>
       </c>
     </row>
     <row r="40">
@@ -3665,13 +3665,13 @@
         <v>74</v>
       </c>
       <c r="C40" t="n">
-        <v>9.86668189981837</v>
+        <v>9.86679157009532</v>
       </c>
       <c r="D40" t="n">
-        <v>4.45164645293173</v>
+        <v>4.45175286378444</v>
       </c>
       <c r="E40" t="n">
-        <v>15.281717346705</v>
+        <v>15.2818302764062</v>
       </c>
     </row>
     <row r="41">
@@ -3682,13 +3682,13 @@
         <v>183</v>
       </c>
       <c r="C41" t="n">
-        <v>0.382419182882089</v>
+        <v>0.381959735153278</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>5.7840158420906</v>
+        <v>5.78356001204901</v>
       </c>
     </row>
     <row r="42">
@@ -3699,13 +3699,13 @@
         <v>76</v>
       </c>
       <c r="C42" t="n">
-        <v>3.3750804549205</v>
+        <v>3.37475102571554</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>8.83881194214171</v>
+        <v>8.83848589635631</v>
       </c>
     </row>
     <row r="43">
@@ -3716,13 +3716,13 @@
         <v>102</v>
       </c>
       <c r="C43" t="n">
-        <v>4.17632757274646</v>
+        <v>4.17625142818695</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>9.58040253632475</v>
+        <v>9.58032989691042</v>
       </c>
     </row>
     <row r="44">
@@ -3733,13 +3733,13 @@
         <v>205</v>
       </c>
       <c r="C44" t="n">
-        <v>0.351192336062621</v>
+        <v>0.351331326813973</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>5.75149939550651</v>
+        <v>5.75162072466845</v>
       </c>
     </row>
     <row r="45">
@@ -3750,13 +3750,13 @@
         <v>173</v>
       </c>
       <c r="C45" t="n">
-        <v>0.37197484676247</v>
+        <v>0.372091975409813</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>5.77357927800047</v>
+        <v>5.77370011861193</v>
       </c>
     </row>
     <row r="46">
@@ -3767,13 +3767,13 @@
         <v>69</v>
       </c>
       <c r="C46" t="n">
-        <v>7.62746565140784</v>
+        <v>7.62757545393359</v>
       </c>
       <c r="D46" t="n">
-        <v>2.2194357831043</v>
+        <v>2.21954189122844</v>
       </c>
       <c r="E46" t="n">
-        <v>13.0354955197114</v>
+        <v>13.0356090166387</v>
       </c>
     </row>
     <row r="47">
@@ -3784,13 +3784,13 @@
         <v>211</v>
       </c>
       <c r="C47" t="n">
-        <v>0.350882648588827</v>
+        <v>0.351021567200955</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>5.75088173949395</v>
+        <v>5.75100292435423</v>
       </c>
     </row>
     <row r="48">
@@ -3801,13 +3801,13 @@
         <v>98</v>
       </c>
       <c r="C48" t="n">
-        <v>1.67732630694362</v>
+        <v>1.67744628562674</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>7.08100807232083</v>
+        <v>7.08113160197031</v>
       </c>
     </row>
     <row r="49">
@@ -3818,13 +3818,13 @@
         <v>209</v>
       </c>
       <c r="C49" t="n">
-        <v>0.350991096919047</v>
+        <v>0.351130038495845</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>5.75109805874929</v>
+        <v>5.75121928954548</v>
       </c>
     </row>
     <row r="50">
@@ -3835,13 +3835,13 @@
         <v>92</v>
       </c>
       <c r="C50" t="n">
-        <v>1.55635622742978</v>
+        <v>1.55647292126358</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>6.9583247079787</v>
+        <v>6.95844511753669</v>
       </c>
     </row>
     <row r="51">
@@ -3852,13 +3852,13 @@
         <v>210</v>
       </c>
       <c r="C51" t="n">
-        <v>0.350929358249242</v>
+        <v>0.351068286752965</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>5.7509749090875</v>
+        <v>5.7510961137337</v>
       </c>
     </row>
     <row r="52">
@@ -3869,13 +3869,13 @@
         <v>80</v>
       </c>
       <c r="C52" t="n">
-        <v>2.41173716686098</v>
+        <v>2.41185440718709</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>7.81374562439363</v>
+        <v>7.81386663047773</v>
       </c>
     </row>
     <row r="53">
@@ -3886,13 +3886,13 @@
         <v>212</v>
       </c>
       <c r="C53" t="n">
-        <v>0.350508619763976</v>
+        <v>0.350668282383311</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>5.73256808496075</v>
+        <v>5.7327080706514</v>
       </c>
     </row>
     <row r="54">
@@ -3903,13 +3903,13 @@
         <v>117</v>
       </c>
       <c r="C54" t="n">
-        <v>1.19476036388767</v>
+        <v>1.19445851675662</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>6.59650846190481</v>
+        <v>6.59621022972341</v>
       </c>
     </row>
     <row r="55">
@@ -3920,13 +3920,13 @@
         <v>108</v>
       </c>
       <c r="C55" t="n">
-        <v>1.02343921606382</v>
+        <v>1.02356050471856</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>6.42516672015954</v>
+        <v>6.42529166258833</v>
       </c>
     </row>
     <row r="56">
@@ -3937,13 +3937,13 @@
         <v>97</v>
       </c>
       <c r="C56" t="n">
-        <v>1.16222079360447</v>
+        <v>1.16235471010136</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>6.5679540447125</v>
+        <v>6.56809169065459</v>
       </c>
     </row>
     <row r="57">
@@ -3954,13 +3954,13 @@
         <v>107</v>
       </c>
       <c r="C57" t="n">
-        <v>1.0637605037067</v>
+        <v>1.06387688172355</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>6.46544632764456</v>
+        <v>6.46556641891846</v>
       </c>
     </row>
     <row r="58">
@@ -3968,16 +3968,16 @@
         <v>2023</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C58" t="n">
-        <v>0.351675247853753</v>
+        <v>0.351814238433637</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>5.75246528786967</v>
+        <v>5.75258661669002</v>
       </c>
     </row>
     <row r="59">
@@ -3988,13 +3988,13 @@
         <v>176</v>
       </c>
       <c r="C59" t="n">
-        <v>0.477676107853913</v>
+        <v>0.477793626689722</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>5.87928952792899</v>
+        <v>5.87941075907908</v>
       </c>
     </row>
     <row r="60">
@@ -4005,13 +4005,13 @@
         <v>118</v>
       </c>
       <c r="C60" t="n">
-        <v>0.808835081824751</v>
+        <v>0.808706035960837</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>6.21044796123754</v>
+        <v>6.21032257452154</v>
       </c>
     </row>
     <row r="61">
@@ -4022,13 +4022,13 @@
         <v>133</v>
       </c>
       <c r="C61" t="n">
-        <v>1.58372958785628</v>
+        <v>1.58383888260237</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>6.98630187082835</v>
+        <v>6.98641487691164</v>
       </c>
     </row>
     <row r="62">
@@ -4039,13 +4039,13 @@
         <v>110</v>
       </c>
       <c r="C62" t="n">
-        <v>3.36778363791619</v>
+        <v>3.36788497237642</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>8.77189027588343</v>
+        <v>8.77199531882086</v>
       </c>
     </row>
     <row r="63">
@@ -4056,13 +4056,13 @@
         <v>33</v>
       </c>
       <c r="C63" t="n">
-        <v>0.350340180395379</v>
+        <v>0.350479166389934</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>5.74979701493359</v>
+        <v>5.74991833462279</v>
       </c>
     </row>
     <row r="64">
@@ -4073,13 +4073,13 @@
         <v>85</v>
       </c>
       <c r="C64" t="n">
-        <v>14.5697523786028</v>
+        <v>14.5695469330398</v>
       </c>
       <c r="D64" t="n">
-        <v>9.1320057305079</v>
+        <v>9.13179770834039</v>
       </c>
       <c r="E64" t="n">
-        <v>20.0074990266977</v>
+        <v>20.0072961577392</v>
       </c>
     </row>
     <row r="65">
@@ -4090,13 +4090,13 @@
         <v>113</v>
       </c>
       <c r="C65" t="n">
-        <v>0.722955344975875</v>
+        <v>0.72174253951607</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>6.12568304798745</v>
+        <v>6.12447370587285</v>
       </c>
     </row>
     <row r="66">
@@ -4107,13 +4107,13 @@
         <v>67</v>
       </c>
       <c r="C66" t="n">
-        <v>35.2644323163677</v>
+        <v>35.2640045817309</v>
       </c>
       <c r="D66" t="n">
-        <v>29.7052207223307</v>
+        <v>29.7047937380649</v>
       </c>
       <c r="E66" t="n">
-        <v>40.8236439104047</v>
+        <v>40.8232154253969</v>
       </c>
     </row>
     <row r="67">
@@ -4121,16 +4121,16 @@
         <v>2023</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C67" t="n">
-        <v>0.364148061613438</v>
+        <v>0.363881822930571</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>5.76574004654146</v>
+        <v>5.76547745941624</v>
       </c>
     </row>
     <row r="68">
@@ -4141,13 +4141,13 @@
         <v>87</v>
       </c>
       <c r="C68" t="n">
-        <v>2.58696219766758</v>
+        <v>2.58708666767925</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>7.99130307333677</v>
+        <v>7.99143127202825</v>
       </c>
     </row>
     <row r="69">
@@ -4158,13 +4158,13 @@
         <v>178</v>
       </c>
       <c r="C69" t="n">
-        <v>0.367578677291465</v>
+        <v>0.367696351385604</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>5.76915435415267</v>
+        <v>5.76927573686633</v>
       </c>
     </row>
     <row r="70">
@@ -4175,13 +4175,13 @@
         <v>109</v>
       </c>
       <c r="C70" t="n">
-        <v>0.741204249696954</v>
+        <v>0.741320727619539</v>
       </c>
       <c r="D70" t="n">
         <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>6.14288957489347</v>
+        <v>6.14300976578597</v>
       </c>
     </row>
     <row r="71">
@@ -4192,13 +4192,13 @@
         <v>148</v>
       </c>
       <c r="C71" t="n">
-        <v>0.872052588414354</v>
+        <v>0.872274509939191</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>6.31954583871957</v>
+        <v>6.31977151486941</v>
       </c>
     </row>
     <row r="72">
@@ -4209,13 +4209,13 @@
         <v>64</v>
       </c>
       <c r="C72" t="n">
-        <v>13.1270264996052</v>
+        <v>13.1271348938662</v>
       </c>
       <c r="D72" t="n">
-        <v>7.70443457819657</v>
+        <v>7.70453925527212</v>
       </c>
       <c r="E72" t="n">
-        <v>18.5496184210137</v>
+        <v>18.5497305324602</v>
       </c>
     </row>
     <row r="73">
@@ -4226,13 +4226,13 @@
         <v>121</v>
       </c>
       <c r="C73" t="n">
-        <v>2.94026721291509</v>
+        <v>2.94038282843953</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>8.34312213228106</v>
+        <v>8.34324146735995</v>
       </c>
     </row>
     <row r="74">
@@ -4243,13 +4243,13 @@
         <v>128</v>
       </c>
       <c r="C74" t="n">
-        <v>0.590454720544708</v>
+        <v>0.590330737586818</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>5.99202060342829</v>
+        <v>5.99190030935153</v>
       </c>
     </row>
     <row r="75">
@@ -4260,13 +4260,13 @@
         <v>125</v>
       </c>
       <c r="C75" t="n">
-        <v>0.829317571213877</v>
+        <v>0.82943717955284</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>6.23087060991109</v>
+        <v>6.23099389168102</v>
       </c>
     </row>
     <row r="76">
@@ -4277,13 +4277,13 @@
         <v>154</v>
       </c>
       <c r="C76" t="n">
-        <v>0.403910479454739</v>
+        <v>0.404028053014986</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
       </c>
       <c r="E76" t="n">
-        <v>5.80551123250384</v>
+        <v>5.80563251814447</v>
       </c>
     </row>
     <row r="77">
@@ -4294,13 +4294,13 @@
         <v>105</v>
       </c>
       <c r="C77" t="n">
-        <v>8.3320113628308</v>
+        <v>8.33212215667245</v>
       </c>
       <c r="D77" t="n">
-        <v>2.92103209897719</v>
+        <v>2.92113916476061</v>
       </c>
       <c r="E77" t="n">
-        <v>13.7429906266844</v>
+        <v>13.7431051485843</v>
       </c>
     </row>
     <row r="78">
@@ -4308,16 +4308,16 @@
         <v>2023</v>
       </c>
       <c r="B78" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C78" t="n">
-        <v>0.351349164499855</v>
+        <v>0.351363150985716</v>
       </c>
       <c r="D78" t="n">
         <v>0</v>
       </c>
       <c r="E78" t="n">
-        <v>5.75181301980606</v>
+        <v>5.75168430163139</v>
       </c>
     </row>
     <row r="79">
@@ -4328,13 +4328,13 @@
         <v>100</v>
       </c>
       <c r="C79" t="n">
-        <v>3.72922877887223</v>
+        <v>3.72893473343752</v>
       </c>
       <c r="D79" t="n">
         <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>9.13538967582114</v>
+        <v>9.13509872621472</v>
       </c>
     </row>
     <row r="80">
@@ -4345,13 +4345,13 @@
         <v>96</v>
       </c>
       <c r="C80" t="n">
-        <v>11.7100896796745</v>
+        <v>11.7101958253832</v>
       </c>
       <c r="D80" t="n">
-        <v>6.27909553036942</v>
+        <v>6.27919794523786</v>
       </c>
       <c r="E80" t="n">
-        <v>17.1410838289796</v>
+        <v>17.1411937055285</v>
       </c>
     </row>
     <row r="81">
@@ -4362,13 +4362,13 @@
         <v>115</v>
       </c>
       <c r="C81" t="n">
-        <v>2.02732202666119</v>
+        <v>2.02743833308626</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
       </c>
       <c r="E81" t="n">
-        <v>7.42953518551988</v>
+        <v>7.42965520901185</v>
       </c>
     </row>
     <row r="82">
@@ -4379,13 +4379,13 @@
         <v>147</v>
       </c>
       <c r="C82" t="n">
-        <v>0.487701771477443</v>
+        <v>0.487819323429912</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
       </c>
       <c r="E82" t="n">
-        <v>5.88930671220677</v>
+        <v>5.8894279759868</v>
       </c>
     </row>
     <row r="83">
@@ -4396,13 +4396,13 @@
         <v>214</v>
       </c>
       <c r="C83" t="n">
-        <v>0.346056469966773</v>
+        <v>0.346194378988225</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>5.74126307801592</v>
+        <v>5.74138224340668</v>
       </c>
     </row>
     <row r="84">
@@ -4419,7 +4419,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>4.58057768291489</v>
+        <v>4.5778543896752</v>
       </c>
     </row>
     <row r="85">
@@ -4430,13 +4430,13 @@
         <v>203</v>
       </c>
       <c r="C85" t="n">
-        <v>0.351224158582765</v>
+        <v>0.351363149511382</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>5.75156296922541</v>
+        <v>5.7516842987402</v>
       </c>
     </row>
     <row r="86">
@@ -4447,13 +4447,13 @@
         <v>93</v>
       </c>
       <c r="C86" t="n">
-        <v>2.05138792078977</v>
+        <v>2.0515040531625</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>7.45377800736172</v>
+        <v>7.45389786788242</v>
       </c>
     </row>
     <row r="87">
@@ -4464,13 +4464,13 @@
         <v>103</v>
       </c>
       <c r="C87" t="n">
-        <v>1.03106201366173</v>
+        <v>1.03117913828874</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>6.43280154572288</v>
+        <v>6.43292238275907</v>
       </c>
     </row>
     <row r="88">
@@ -4481,13 +4481,13 @@
         <v>81</v>
       </c>
       <c r="C88" t="n">
-        <v>3.90585834259147</v>
+        <v>3.90305921255879</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>9.31009103149437</v>
+        <v>9.30729219922741</v>
       </c>
     </row>
     <row r="89">
@@ -4498,13 +4498,13 @@
         <v>161</v>
       </c>
       <c r="C89" t="n">
-        <v>0.536217824648182</v>
+        <v>0.53633519029735</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>5.93784407107721</v>
+        <v>5.93796514921397</v>
       </c>
     </row>
     <row r="90">
@@ -4515,13 +4515,13 @@
         <v>77</v>
       </c>
       <c r="C90" t="n">
-        <v>5.44788100826755</v>
+        <v>5.44736770626862</v>
       </c>
       <c r="D90" t="n">
-        <v>0.119071541183303</v>
+        <v>0.118867283933843</v>
       </c>
       <c r="E90" t="n">
-        <v>10.8758395399855</v>
+        <v>10.8753318677517</v>
       </c>
     </row>
     <row r="91">
@@ -4532,13 +4532,13 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>1.56811137910817</v>
+        <v>1.56798287266499</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>6.96987395239306</v>
+        <v>6.9697490983336</v>
       </c>
     </row>
     <row r="92">
@@ -4549,13 +4549,13 @@
         <v>156</v>
       </c>
       <c r="C92" t="n">
-        <v>0.582069638711232</v>
+        <v>0.58218701968462</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>5.98372067728988</v>
+        <v>5.98384177116119</v>
       </c>
     </row>
     <row r="93">
@@ -4566,13 +4566,13 @@
         <v>179</v>
       </c>
       <c r="C93" t="n">
-        <v>0.413690516066874</v>
+        <v>0.413807690194662</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>5.81531023531599</v>
+        <v>5.81543112172139</v>
       </c>
     </row>
     <row r="94">
@@ -4580,16 +4580,16 @@
         <v>2023</v>
       </c>
       <c r="B94" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C94" t="n">
-        <v>0.351590894405607</v>
+        <v>0.351682359548034</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>5.75229655475843</v>
+        <v>5.75232281793648</v>
       </c>
     </row>
     <row r="95">
@@ -4600,13 +4600,13 @@
         <v>155</v>
       </c>
       <c r="C95" t="n">
-        <v>0.440909401670528</v>
+        <v>0.441026999877089</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>5.84249476314405</v>
+        <v>5.8426160701386</v>
       </c>
     </row>
     <row r="96">
@@ -4617,13 +4617,13 @@
         <v>116</v>
       </c>
       <c r="C96" t="n">
-        <v>0.949441462484605</v>
+        <v>0.949561063682757</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>6.35212190516224</v>
+        <v>6.35224510218986</v>
       </c>
     </row>
     <row r="97">
@@ -4634,13 +4634,13 @@
         <v>215</v>
       </c>
       <c r="C97" t="n">
-        <v>0.0791793371196524</v>
+        <v>0.0793168096193734</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>5.21006482034259</v>
+        <v>5.21018312386222</v>
       </c>
     </row>
     <row r="98">
@@ -4651,13 +4651,13 @@
         <v>84</v>
       </c>
       <c r="C98" t="n">
-        <v>3.51999761506847</v>
+        <v>3.52012057259247</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>8.93457907988448</v>
+        <v>8.93470537423437</v>
       </c>
     </row>
     <row r="99">
@@ -4668,13 +4668,13 @@
         <v>157</v>
       </c>
       <c r="C99" t="n">
-        <v>0.380371996528178</v>
+        <v>0.380489623526309</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>5.78195718750302</v>
+        <v>5.7820785238053</v>
       </c>
     </row>
     <row r="100">
@@ -4685,13 +4685,13 @@
         <v>158</v>
       </c>
       <c r="C100" t="n">
-        <v>0.415890655431748</v>
+        <v>0.416007691726492</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>5.81748251859473</v>
+        <v>5.81760326398577</v>
       </c>
     </row>
     <row r="101">
@@ -4702,13 +4702,13 @@
         <v>106</v>
       </c>
       <c r="C101" t="n">
-        <v>3.34633504529754</v>
+        <v>3.34611841477624</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>8.74920386961241</v>
+        <v>8.74899077657133</v>
       </c>
     </row>
     <row r="102">
@@ -4719,13 +4719,13 @@
         <v>207</v>
       </c>
       <c r="C102" t="n">
-        <v>0.351121651112203</v>
+        <v>0.351260641468633</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>5.75135818430318</v>
+        <v>5.7514795126785</v>
       </c>
     </row>
     <row r="103">
@@ -4736,13 +4736,13 @@
         <v>123</v>
       </c>
       <c r="C103" t="n">
-        <v>1.66042501518306</v>
+        <v>1.65987219885768</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>7.06247932916821</v>
+        <v>7.06192990846211</v>
       </c>
     </row>
     <row r="104">
@@ -4753,13 +4753,13 @@
         <v>65</v>
       </c>
       <c r="C104" t="n">
-        <v>10.3963298191726</v>
+        <v>10.3962004530635</v>
       </c>
       <c r="D104" t="n">
-        <v>4.98352765598146</v>
+        <v>4.98339517453647</v>
       </c>
       <c r="E104" t="n">
-        <v>15.8091319823637</v>
+        <v>15.8090057315906</v>
       </c>
     </row>
     <row r="105">
@@ -4770,13 +4770,13 @@
         <v>165</v>
       </c>
       <c r="C105" t="n">
-        <v>0.363416099584635</v>
+        <v>0.363535497305675</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>5.76524792671432</v>
+        <v>5.76537103520373</v>
       </c>
     </row>
     <row r="106">
@@ -4787,13 +4787,13 @@
         <v>63</v>
       </c>
       <c r="C106" t="n">
-        <v>19.1086060468656</v>
+        <v>19.1086311017605</v>
       </c>
       <c r="D106" t="n">
-        <v>13.6574912182851</v>
+        <v>13.6575129109481</v>
       </c>
       <c r="E106" t="n">
-        <v>24.5597208754462</v>
+        <v>24.559749292573</v>
       </c>
     </row>
     <row r="107">
@@ -4804,13 +4804,13 @@
         <v>122</v>
       </c>
       <c r="C107" t="n">
-        <v>0.770834812874496</v>
+        <v>0.769105124157483</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>6.17241575409594</v>
+        <v>6.17068952523627</v>
       </c>
     </row>
     <row r="108">
@@ -4821,13 +4821,13 @@
         <v>191</v>
       </c>
       <c r="C108" t="n">
-        <v>0.351783907721728</v>
+        <v>0.351875372714931</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>5.75268264138516</v>
+        <v>5.75270890425659</v>
       </c>
     </row>
     <row r="109">
@@ -4838,13 +4838,13 @@
         <v>163</v>
       </c>
       <c r="C109" t="n">
-        <v>0.380198986097252</v>
+        <v>0.380316580356879</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>5.78179528291233</v>
+        <v>5.78191658916356</v>
       </c>
     </row>
     <row r="110">
@@ -4852,16 +4852,16 @@
         <v>2023</v>
       </c>
       <c r="B110" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C110" t="n">
-        <v>0.351390415087983</v>
+        <v>0.351529405188472</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>5.75189555173621</v>
+        <v>5.75201687959555</v>
       </c>
     </row>
     <row r="111">
@@ -4872,13 +4872,13 @@
         <v>114</v>
       </c>
       <c r="C111" t="n">
-        <v>0.864925494092157</v>
+        <v>0.865061822096548</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>6.26822784913354</v>
+        <v>6.26836792309186</v>
       </c>
     </row>
     <row r="112">
@@ -4889,13 +4889,13 @@
         <v>71</v>
       </c>
       <c r="C112" t="n">
-        <v>5.24236837869737</v>
+        <v>5.24247644051913</v>
       </c>
       <c r="D112" t="n">
-        <v>0.0924983231637519</v>
+        <v>0.0926305522979338</v>
       </c>
       <c r="E112" t="n">
-        <v>10.6479929804153</v>
+        <v>10.6481047608068</v>
       </c>
     </row>
     <row r="113">
@@ -4906,13 +4906,13 @@
         <v>112</v>
       </c>
       <c r="C113" t="n">
-        <v>0.741338864613219</v>
+        <v>0.741455946430002</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>6.1430150215273</v>
+        <v>6.14313581648079</v>
       </c>
     </row>
     <row r="114">
@@ -4923,13 +4923,13 @@
         <v>190</v>
       </c>
       <c r="C114" t="n">
-        <v>0.359830767508358</v>
+        <v>0.359948377512569</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>5.76142379878581</v>
+        <v>5.76154512071346</v>
       </c>
     </row>
     <row r="115">
@@ -4940,13 +4940,13 @@
         <v>134</v>
       </c>
       <c r="C115" t="n">
-        <v>0.476744885083813</v>
+        <v>0.476862569783208</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>5.87834151323066</v>
+        <v>5.87846291665301</v>
       </c>
     </row>
     <row r="116">
@@ -4954,16 +4954,16 @@
         <v>2023</v>
       </c>
       <c r="B116" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C116" t="n">
-        <v>0.351637087915529</v>
+        <v>0.351775871853511</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>5.75239563131991</v>
+        <v>5.75251654680974</v>
       </c>
     </row>
     <row r="117">
@@ -4974,13 +4974,13 @@
         <v>182</v>
       </c>
       <c r="C117" t="n">
-        <v>0.352353547784881</v>
+        <v>0.352492537840346</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>5.75382209879619</v>
+        <v>5.75394342657232</v>
       </c>
     </row>
     <row r="118">
@@ -4991,13 +4991,13 @@
         <v>89</v>
       </c>
       <c r="C118" t="n">
-        <v>2.04092403045827</v>
+        <v>2.04104377306428</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>7.44500962096123</v>
+        <v>7.44513321143334</v>
       </c>
     </row>
     <row r="119">
@@ -5008,13 +5008,13 @@
         <v>130</v>
       </c>
       <c r="C119" t="n">
-        <v>0.618834272272058</v>
+        <v>0.618796500288817</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>6.02047158529564</v>
+        <v>6.02043748926525</v>
       </c>
     </row>
     <row r="120">
@@ -5025,13 +5025,13 @@
         <v>206</v>
       </c>
       <c r="C120" t="n">
-        <v>0.351167498201752</v>
+        <v>0.351306487194202</v>
       </c>
       <c r="D120" t="n">
         <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>5.75145042937807</v>
+        <v>5.7515717550367</v>
       </c>
     </row>
     <row r="121">
@@ -5042,13 +5042,13 @@
         <v>171</v>
       </c>
       <c r="C121" t="n">
-        <v>0.370987028371623</v>
+        <v>0.371104629751939</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>5.77258183508102</v>
+        <v>5.77270314842213</v>
       </c>
     </row>
     <row r="122">
@@ -5059,13 +5059,13 @@
         <v>162</v>
       </c>
       <c r="C122" t="n">
-        <v>0.633082099107899</v>
+        <v>0.633199402937339</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>6.03475775329815</v>
+        <v>6.03487877034803</v>
       </c>
     </row>
     <row r="123">
@@ -5076,13 +5076,13 @@
         <v>75</v>
       </c>
       <c r="C123" t="n">
-        <v>8.78062308879075</v>
+        <v>8.77999870373587</v>
       </c>
       <c r="D123" t="n">
-        <v>3.16897695189537</v>
+        <v>3.16856939214101</v>
       </c>
       <c r="E123" t="n">
-        <v>14.4108802416391</v>
+        <v>14.4102657119829</v>
       </c>
     </row>
     <row r="124">
@@ -5093,13 +5093,13 @@
         <v>152</v>
       </c>
       <c r="C124" t="n">
-        <v>0.803763861237097</v>
+        <v>0.803880776853297</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>6.20545677246324</v>
+        <v>6.20557740137212</v>
       </c>
     </row>
     <row r="125">
@@ -5110,13 +5110,13 @@
         <v>78</v>
       </c>
       <c r="C125" t="n">
-        <v>3.88017596106416</v>
+        <v>3.88029058276567</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>9.28402224243539</v>
+        <v>9.28414058792184</v>
       </c>
     </row>
     <row r="126">
@@ -5124,16 +5124,16 @@
         <v>2023</v>
       </c>
       <c r="B126" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C126" t="n">
-        <v>0.351740607731796</v>
+        <v>0.351879598242447</v>
       </c>
       <c r="D126" t="n">
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>5.75259602842428</v>
+        <v>5.7527173571065</v>
       </c>
     </row>
     <row r="127">
@@ -5144,13 +5144,13 @@
         <v>204</v>
       </c>
       <c r="C127" t="n">
-        <v>0.351224158582752</v>
+        <v>0.351363149511354</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>5.75156296922537</v>
+        <v>5.75168429874012</v>
       </c>
     </row>
     <row r="128">
@@ -5161,13 +5161,13 @@
         <v>167</v>
       </c>
       <c r="C128" t="n">
-        <v>0.398664138756837</v>
+        <v>0.398777800851818</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
       </c>
       <c r="E128" t="n">
-        <v>5.80033513936972</v>
+        <v>5.8004525186643</v>
       </c>
     </row>
     <row r="129">
@@ -5178,13 +5178,13 @@
         <v>201</v>
       </c>
       <c r="C129" t="n">
-        <v>0.351224158877173</v>
+        <v>0.351363149806233</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>5.75156296980282</v>
+        <v>5.75168429931847</v>
       </c>
     </row>
     <row r="130">
@@ -5195,13 +5195,13 @@
         <v>172</v>
       </c>
       <c r="C130" t="n">
-        <v>0.509208342997091</v>
+        <v>0.509325837543411</v>
       </c>
       <c r="D130" t="n">
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>5.91082779791288</v>
+        <v>5.91094900487699</v>
       </c>
     </row>
     <row r="131">
@@ -5212,13 +5212,13 @@
         <v>120</v>
       </c>
       <c r="C131" t="n">
-        <v>0.743595324611903</v>
+        <v>0.743712679540359</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>6.14525709913769</v>
+        <v>6.14537816905731</v>
       </c>
     </row>
     <row r="132">
@@ -5229,13 +5229,13 @@
         <v>111</v>
       </c>
       <c r="C132" t="n">
-        <v>0.742967615658048</v>
+        <v>0.741696099956548</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>6.14464923461451</v>
+        <v>6.14338115661957</v>
       </c>
     </row>
     <row r="133">
@@ -5246,13 +5246,13 @@
         <v>168</v>
       </c>
       <c r="C133" t="n">
-        <v>0.370761718250423</v>
+        <v>0.370879355774493</v>
       </c>
       <c r="D133" t="n">
         <v>0</v>
       </c>
       <c r="E133" t="n">
-        <v>5.77234647500485</v>
+        <v>5.77246782278049</v>
       </c>
     </row>
     <row r="134">
@@ -5263,13 +5263,13 @@
         <v>180</v>
       </c>
       <c r="C134" t="n">
-        <v>0.352447895059809</v>
+        <v>0.352586848106566</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>5.75401177741423</v>
+        <v>5.75413303116374</v>
       </c>
     </row>
     <row r="135">
@@ -5280,13 +5280,13 @@
         <v>174</v>
       </c>
       <c r="C135" t="n">
-        <v>0.394378274392442</v>
+        <v>0.394233856918293</v>
       </c>
       <c r="D135" t="n">
         <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>5.79598277734412</v>
+        <v>5.79584202701592</v>
       </c>
     </row>
     <row r="136">
@@ -5297,13 +5297,13 @@
         <v>169</v>
       </c>
       <c r="C136" t="n">
-        <v>0.371033045720286</v>
+        <v>0.371150647065111</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>5.77262785981923</v>
+        <v>5.772749173125</v>
       </c>
     </row>
     <row r="137">
@@ -5314,13 +5314,13 @@
         <v>202</v>
       </c>
       <c r="C137" t="n">
-        <v>0.351224158711744</v>
+        <v>0.351363149640497</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>5.75156296947826</v>
+        <v>5.75168429899331</v>
       </c>
     </row>
     <row r="138">
@@ -5331,13 +5331,13 @@
         <v>119</v>
       </c>
       <c r="C138" t="n">
-        <v>0.574114515638773</v>
+        <v>0.573970569216621</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>5.97574994364318</v>
+        <v>5.97560965414986</v>
       </c>
     </row>
     <row r="139">
@@ -5348,13 +5348,13 @@
         <v>181</v>
       </c>
       <c r="C139" t="n">
-        <v>0.391897475298288</v>
+        <v>0.392053177830799</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>5.75982443004635</v>
+        <v>5.75995591132182</v>
       </c>
     </row>
     <row r="140">
@@ -5365,13 +5365,13 @@
         <v>73</v>
       </c>
       <c r="C140" t="n">
-        <v>6.06388775941671</v>
+        <v>6.06400294138586</v>
       </c>
       <c r="D140" t="n">
-        <v>0.659813199553109</v>
+        <v>0.659924575756894</v>
       </c>
       <c r="E140" t="n">
-        <v>11.4679623192803</v>
+        <v>11.4680813070148</v>
       </c>
     </row>
     <row r="141">
@@ -5382,13 +5382,13 @@
         <v>28</v>
       </c>
       <c r="C141" t="n">
-        <v>0.372953693864616</v>
+        <v>0.372083464200109</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>5.77454893214543</v>
+        <v>5.77368225527167</v>
       </c>
     </row>
     <row r="142">
@@ -5399,13 +5399,13 @@
         <v>189</v>
       </c>
       <c r="C142" t="n">
-        <v>0.351853319561139</v>
+        <v>0.351992310003451</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>5.7528214866487</v>
+        <v>5.75294281519505</v>
       </c>
     </row>
     <row r="143">
@@ -5416,13 +5416,13 @@
         <v>131</v>
       </c>
       <c r="C143" t="n">
-        <v>0.644970245749334</v>
+        <v>0.645087799094485</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>6.0465503823176</v>
+        <v>6.0466716376752</v>
       </c>
     </row>
     <row r="144">
@@ -5433,13 +5433,13 @@
         <v>94</v>
       </c>
       <c r="C144" t="n">
-        <v>2.27666277560421</v>
+        <v>2.27677903405397</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>7.67879020944036</v>
+        <v>7.67891017097592</v>
       </c>
     </row>
     <row r="145">
@@ -5450,13 +5450,13 @@
         <v>68</v>
       </c>
       <c r="C145" t="n">
-        <v>15.4531973936244</v>
+        <v>15.4534442428658</v>
       </c>
       <c r="D145" t="n">
-        <v>9.33347850303218</v>
+        <v>9.3337257789946</v>
       </c>
       <c r="E145" t="n">
-        <v>21.5729162842167</v>
+        <v>21.5731627067371</v>
       </c>
     </row>
     <row r="146">
@@ -5467,13 +5467,13 @@
         <v>177</v>
       </c>
       <c r="C146" t="n">
-        <v>0.464483547942825</v>
+        <v>0.46463580657391</v>
       </c>
       <c r="D146" t="n">
         <v>0</v>
       </c>
       <c r="E146" t="n">
-        <v>5.78864757660235</v>
+        <v>5.78875720878672</v>
       </c>
     </row>
     <row r="147">
@@ -5484,13 +5484,13 @@
         <v>66</v>
       </c>
       <c r="C147" t="n">
-        <v>15.8599470531149</v>
+        <v>15.8599287419729</v>
       </c>
       <c r="D147" t="n">
-        <v>10.1831559563057</v>
+        <v>10.1831340658768</v>
       </c>
       <c r="E147" t="n">
-        <v>21.5367381499242</v>
+        <v>21.5367234180689</v>
       </c>
     </row>
     <row r="148">
@@ -5498,16 +5498,16 @@
         <v>2023</v>
       </c>
       <c r="B148" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C148" t="n">
-        <v>0.359651705256503</v>
+        <v>0.359208276870947</v>
       </c>
       <c r="D148" t="n">
         <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>5.76124377630555</v>
+        <v>5.76080397321006</v>
       </c>
     </row>
     <row r="149">
@@ -5518,13 +5518,13 @@
         <v>101</v>
       </c>
       <c r="C149" t="n">
-        <v>2.40620351374928</v>
+        <v>2.40598657740704</v>
       </c>
       <c r="D149" t="n">
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>7.80945943246979</v>
+        <v>7.80924592199468</v>
       </c>
     </row>
     <row r="150">
@@ -5532,16 +5532,16 @@
         <v>2023</v>
       </c>
       <c r="B150" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C150" t="n">
-        <v>0.353581416178614</v>
+        <v>0.353720416557028</v>
       </c>
       <c r="D150" t="n">
         <v>0</v>
       </c>
       <c r="E150" t="n">
-        <v>5.75482743661964</v>
+        <v>5.75494877648021</v>
       </c>
     </row>
     <row r="151">
@@ -5552,13 +5552,13 @@
         <v>170</v>
       </c>
       <c r="C151" t="n">
-        <v>0.544903180670939</v>
+        <v>0.545020589416799</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>5.94654598320996</v>
+        <v>5.94666710473723</v>
       </c>
     </row>
     <row r="152">
@@ -5569,13 +5569,13 @@
         <v>164</v>
       </c>
       <c r="C152" t="n">
-        <v>0.457019885487038</v>
+        <v>0.457035333370248</v>
       </c>
       <c r="D152" t="n">
         <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>5.85864145568265</v>
+        <v>5.85866059747483</v>
       </c>
     </row>
     <row r="153">
@@ -5583,16 +5583,16 @@
         <v>2023</v>
       </c>
       <c r="B153" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C153" t="n">
-        <v>0.355730621671865</v>
+        <v>0.355848229333532</v>
       </c>
       <c r="D153" t="n">
         <v>0</v>
       </c>
       <c r="E153" t="n">
-        <v>5.75732307895291</v>
+        <v>5.75744439852379</v>
       </c>
     </row>
     <row r="154">
@@ -5603,13 +5603,13 @@
         <v>79</v>
       </c>
       <c r="C154" t="n">
-        <v>4.02736541040689</v>
+        <v>4.02748564408761</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>9.4345700070102</v>
+        <v>9.43469417046462</v>
       </c>
     </row>
     <row r="155">
@@ -5620,13 +5620,13 @@
         <v>88</v>
       </c>
       <c r="C155" t="n">
-        <v>5.90707845279174</v>
+        <v>5.90718685460533</v>
       </c>
       <c r="D155" t="n">
-        <v>0.502290806991711</v>
+        <v>0.502395507214288</v>
       </c>
       <c r="E155" t="n">
-        <v>11.3118660985918</v>
+        <v>11.3119782019964</v>
       </c>
     </row>
     <row r="156">
@@ -5637,13 +5637,13 @@
         <v>141</v>
       </c>
       <c r="C156" t="n">
-        <v>0.529008445719304</v>
+        <v>0.529125880279028</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>5.93059095502359</v>
+        <v>5.93071209512193</v>
       </c>
     </row>
     <row r="157">
@@ -5654,13 +5654,13 @@
         <v>150</v>
       </c>
       <c r="C157" t="n">
-        <v>0.45744933764333</v>
+        <v>0.457566987977717</v>
       </c>
       <c r="D157" t="n">
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>5.85903982812112</v>
+        <v>5.85916118780809</v>
       </c>
     </row>
   </sheetData>
@@ -5702,13 +5702,13 @@
         <v>2023</v>
       </c>
       <c r="C2" t="n">
-        <v>148.491994618902</v>
+        <v>148.477713545171</v>
       </c>
       <c r="D2" t="n">
-        <v>54.6132095012699</v>
+        <v>54.6118669262094</v>
       </c>
       <c r="E2" t="n">
-        <v>572.019306400588</v>
+        <v>572.002557274095</v>
       </c>
     </row>
     <row r="3">
@@ -5719,13 +5719,13 @@
         <v>2023</v>
       </c>
       <c r="C3" t="n">
-        <v>206.750031026826</v>
+        <v>206.759931431922</v>
       </c>
       <c r="D3" t="n">
-        <v>61.4534054733361</v>
+        <v>61.4551396373838</v>
       </c>
       <c r="E3" t="n">
-        <v>632.239401221659</v>
+        <v>632.248304376331</v>
       </c>
     </row>
   </sheetData>
@@ -5758,7 +5758,7 @@
         <v>2018</v>
       </c>
       <c r="B2" t="n">
-        <v>235.587036</v>
+        <v>235.549082</v>
       </c>
       <c r="C2" t="n">
         <v>136.421668</v>
@@ -5802,7 +5802,7 @@
         <v>2022</v>
       </c>
       <c r="B6" t="n">
-        <v>107.749275</v>
+        <v>107.748986</v>
       </c>
       <c r="C6" t="n">
         <v>121.786061</v>
@@ -5813,10 +5813,10 @@
         <v>2023</v>
       </c>
       <c r="B7" t="n">
-        <v>148.491994618902</v>
+        <v>148.477713545171</v>
       </c>
       <c r="C7" t="n">
-        <v>206.750031026826</v>
+        <v>206.759931431922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>